<commit_message>
Deploying to gh-pages from  @ 66dc58de584c843ee1ad6762dfb3b0a2e5106a24 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_5-2-2.xlsx
+++ b/assets/excel/2021_5-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BBE8E5-6F20-44F5-B6C0-E558F35AD0B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9300CCBF-8E72-4810-AA43-8EB3E5734C04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,13 +34,6 @@
   </si>
   <si>
     <t>AGS</t>
-  </si>
-  <si>
-    <t>Kreisfreie Stadt
-Landkreis
-(Großstadt, Umland)
-Statistische Region
-Land</t>
   </si>
   <si>
     <t>Sozialversicherungspflichtig
@@ -115,6 +108,14 @@
   </si>
   <si>
     <t>Tabelle 5.2.2: Sozialversicherungspflichtig Beschäftigte Ausländerinnen und Ausländer am Arbeitsort nach Qualifikation und Kreisen</t>
+  </si>
+  <si>
+    <t>Kreisfreie Stadt
+Landkreis
+(Großstadt, Umland)
+Statistische Region
+Land
+Land</t>
   </si>
 </sst>
 </file>
@@ -505,6 +506,42 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,42 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1444,7 +1445,7 @@
     <row r="2" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -1482,7 +1483,7 @@
     </row>
     <row r="4" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
@@ -1667,552 +1668,552 @@
       <c r="BV6" s="9"/>
     </row>
     <row r="7" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="75">
+      <c r="C7" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="87">
         <v>2020</v>
       </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="75">
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="87">
         <v>2019</v>
       </c>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="75">
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="87">
         <v>2018</v>
       </c>
-      <c r="S7" s="76"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="76"/>
-      <c r="V7" s="76"/>
-      <c r="W7" s="76"/>
-      <c r="X7" s="77"/>
-      <c r="Y7" s="65">
+      <c r="S7" s="88"/>
+      <c r="T7" s="88"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="89"/>
+      <c r="Y7" s="77">
         <v>2017</v>
       </c>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="66"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
-      <c r="AE7" s="67"/>
-      <c r="AF7" s="65">
+      <c r="Z7" s="78"/>
+      <c r="AA7" s="78"/>
+      <c r="AB7" s="78"/>
+      <c r="AC7" s="78"/>
+      <c r="AD7" s="78"/>
+      <c r="AE7" s="79"/>
+      <c r="AF7" s="77">
         <v>2016</v>
       </c>
-      <c r="AG7" s="66"/>
-      <c r="AH7" s="66"/>
-      <c r="AI7" s="66"/>
-      <c r="AJ7" s="66"/>
-      <c r="AK7" s="66"/>
-      <c r="AL7" s="67"/>
-      <c r="AM7" s="65">
+      <c r="AG7" s="78"/>
+      <c r="AH7" s="78"/>
+      <c r="AI7" s="78"/>
+      <c r="AJ7" s="78"/>
+      <c r="AK7" s="78"/>
+      <c r="AL7" s="79"/>
+      <c r="AM7" s="77">
         <v>2015</v>
       </c>
-      <c r="AN7" s="66"/>
-      <c r="AO7" s="66"/>
-      <c r="AP7" s="66"/>
-      <c r="AQ7" s="66"/>
-      <c r="AR7" s="66"/>
-      <c r="AS7" s="67"/>
-      <c r="AT7" s="65">
+      <c r="AN7" s="78"/>
+      <c r="AO7" s="78"/>
+      <c r="AP7" s="78"/>
+      <c r="AQ7" s="78"/>
+      <c r="AR7" s="78"/>
+      <c r="AS7" s="79"/>
+      <c r="AT7" s="77">
         <v>2014</v>
       </c>
-      <c r="AU7" s="66"/>
-      <c r="AV7" s="66"/>
-      <c r="AW7" s="66"/>
-      <c r="AX7" s="66"/>
-      <c r="AY7" s="66"/>
-      <c r="AZ7" s="67"/>
-      <c r="BA7" s="65">
+      <c r="AU7" s="78"/>
+      <c r="AV7" s="78"/>
+      <c r="AW7" s="78"/>
+      <c r="AX7" s="78"/>
+      <c r="AY7" s="78"/>
+      <c r="AZ7" s="79"/>
+      <c r="BA7" s="77">
         <v>2013</v>
       </c>
-      <c r="BB7" s="66"/>
-      <c r="BC7" s="66"/>
-      <c r="BD7" s="66"/>
-      <c r="BE7" s="66"/>
-      <c r="BF7" s="66"/>
-      <c r="BG7" s="67"/>
-      <c r="BH7" s="65">
+      <c r="BB7" s="78"/>
+      <c r="BC7" s="78"/>
+      <c r="BD7" s="78"/>
+      <c r="BE7" s="78"/>
+      <c r="BF7" s="78"/>
+      <c r="BG7" s="79"/>
+      <c r="BH7" s="77">
         <v>2011</v>
       </c>
-      <c r="BI7" s="66"/>
-      <c r="BJ7" s="66"/>
-      <c r="BK7" s="66"/>
-      <c r="BL7" s="66"/>
-      <c r="BM7" s="66"/>
-      <c r="BN7" s="67"/>
-      <c r="BO7" s="68">
+      <c r="BI7" s="78"/>
+      <c r="BJ7" s="78"/>
+      <c r="BK7" s="78"/>
+      <c r="BL7" s="78"/>
+      <c r="BM7" s="78"/>
+      <c r="BN7" s="79"/>
+      <c r="BO7" s="80">
         <v>2010</v>
       </c>
-      <c r="BP7" s="68"/>
-      <c r="BQ7" s="68"/>
-      <c r="BR7" s="68"/>
-      <c r="BS7" s="68"/>
-      <c r="BT7" s="68"/>
-      <c r="BU7" s="65"/>
+      <c r="BP7" s="80"/>
+      <c r="BQ7" s="80"/>
+      <c r="BR7" s="80"/>
+      <c r="BS7" s="80"/>
+      <c r="BT7" s="80"/>
+      <c r="BU7" s="77"/>
       <c r="BV7" s="11"/>
     </row>
-    <row r="8" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="70"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="78" t="s">
+    <row r="8" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="82"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="81" t="s">
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="O8" s="79"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="81" t="s">
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="V8" s="79"/>
-      <c r="W8" s="79"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="85" t="s">
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="Z8" s="85"/>
-      <c r="AA8" s="85"/>
-      <c r="AB8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="84"/>
-      <c r="AF8" s="85" t="s">
+      <c r="AC8" s="70"/>
+      <c r="AD8" s="70"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="68"/>
+      <c r="AH8" s="68"/>
+      <c r="AI8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AG8" s="85"/>
-      <c r="AH8" s="85"/>
-      <c r="AI8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ8" s="83"/>
-      <c r="AK8" s="83"/>
-      <c r="AL8" s="84"/>
-      <c r="AM8" s="85" t="s">
+      <c r="AJ8" s="70"/>
+      <c r="AK8" s="70"/>
+      <c r="AL8" s="67"/>
+      <c r="AM8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN8" s="68"/>
+      <c r="AO8" s="68"/>
+      <c r="AP8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AN8" s="85"/>
-      <c r="AO8" s="85"/>
-      <c r="AP8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="AQ8" s="83"/>
-      <c r="AR8" s="83"/>
-      <c r="AS8" s="84"/>
-      <c r="AT8" s="85" t="s">
+      <c r="AQ8" s="70"/>
+      <c r="AR8" s="70"/>
+      <c r="AS8" s="67"/>
+      <c r="AT8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU8" s="68"/>
+      <c r="AV8" s="68"/>
+      <c r="AW8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AU8" s="85"/>
-      <c r="AV8" s="85"/>
-      <c r="AW8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX8" s="83"/>
-      <c r="AY8" s="83"/>
-      <c r="AZ8" s="84"/>
-      <c r="BA8" s="85" t="s">
+      <c r="AX8" s="70"/>
+      <c r="AY8" s="70"/>
+      <c r="AZ8" s="67"/>
+      <c r="BA8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB8" s="68"/>
+      <c r="BC8" s="68"/>
+      <c r="BD8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BB8" s="85"/>
-      <c r="BC8" s="85"/>
-      <c r="BD8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE8" s="83"/>
-      <c r="BF8" s="83"/>
-      <c r="BG8" s="84"/>
-      <c r="BH8" s="85" t="s">
+      <c r="BE8" s="70"/>
+      <c r="BF8" s="70"/>
+      <c r="BG8" s="67"/>
+      <c r="BH8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI8" s="68"/>
+      <c r="BJ8" s="68"/>
+      <c r="BK8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BI8" s="85"/>
-      <c r="BJ8" s="85"/>
-      <c r="BK8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="BL8" s="83"/>
-      <c r="BM8" s="83"/>
-      <c r="BN8" s="84"/>
-      <c r="BO8" s="86" t="s">
+      <c r="BL8" s="70"/>
+      <c r="BM8" s="70"/>
+      <c r="BN8" s="67"/>
+      <c r="BO8" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP8" s="72"/>
+      <c r="BQ8" s="72"/>
+      <c r="BR8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BP8" s="86"/>
-      <c r="BQ8" s="86"/>
-      <c r="BR8" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="BS8" s="83"/>
-      <c r="BT8" s="83"/>
-      <c r="BU8" s="83"/>
+      <c r="BS8" s="70"/>
+      <c r="BT8" s="70"/>
+      <c r="BU8" s="70"/>
       <c r="BV8" s="9"/>
     </row>
     <row r="9" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="70"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="J9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="K9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="M9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="N9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="O9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="P9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="Q9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="R9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S9" s="12" t="s">
+      <c r="T9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="U9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="U9" s="12" t="s">
+      <c r="V9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="V9" s="12" t="s">
+      <c r="W9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="W9" s="12" t="s">
+      <c r="X9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="X9" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="Y9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Z9" s="13" t="s">
+      <c r="AA9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AA9" s="13" t="s">
+      <c r="AB9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AB9" s="13" t="s">
+      <c r="AC9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AC9" s="13" t="s">
+      <c r="AD9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AD9" s="13" t="s">
+      <c r="AE9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AE9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="AF9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AG9" s="13" t="s">
+      <c r="AH9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AH9" s="13" t="s">
+      <c r="AI9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AI9" s="13" t="s">
+      <c r="AJ9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AJ9" s="13" t="s">
+      <c r="AK9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AK9" s="13" t="s">
+      <c r="AL9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AL9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="AM9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AN9" s="13" t="s">
+      <c r="AO9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AO9" s="13" t="s">
+      <c r="AP9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AP9" s="13" t="s">
+      <c r="AQ9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AQ9" s="13" t="s">
+      <c r="AR9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AR9" s="13" t="s">
+      <c r="AS9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AS9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="AT9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AU9" s="13" t="s">
+      <c r="AV9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AV9" s="13" t="s">
+      <c r="AW9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AW9" s="13" t="s">
+      <c r="AX9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AX9" s="13" t="s">
+      <c r="AY9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AY9" s="13" t="s">
+      <c r="AZ9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AZ9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="BA9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="BB9" s="13" t="s">
+      <c r="BC9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="BC9" s="13" t="s">
+      <c r="BD9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="BD9" s="13" t="s">
+      <c r="BE9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="BE9" s="13" t="s">
+      <c r="BF9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="BF9" s="13" t="s">
+      <c r="BG9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="BG9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="BH9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="BI9" s="13" t="s">
+      <c r="BJ9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="BJ9" s="13" t="s">
+      <c r="BK9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="BK9" s="13" t="s">
+      <c r="BL9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="BL9" s="13" t="s">
+      <c r="BM9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="BM9" s="13" t="s">
+      <c r="BN9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="BN9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="BO9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="BP9" s="13" t="s">
+      <c r="BQ9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="BQ9" s="13" t="s">
+      <c r="BR9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="BR9" s="13" t="s">
+      <c r="BS9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="BS9" s="13" t="s">
+      <c r="BT9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="BT9" s="14" t="s">
+      <c r="BU9" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="BU9" s="14" t="s">
-        <v>11</v>
       </c>
       <c r="BV9" s="9"/>
     </row>
     <row r="10" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="71"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="78" t="s">
+      <c r="B10" s="83"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="79"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="81" t="s">
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" s="81"/>
-      <c r="P10" s="78"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="73"/>
       <c r="Q10" s="15"/>
-      <c r="R10" s="81" t="s">
+      <c r="R10" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="V10" s="81"/>
-      <c r="W10" s="78"/>
+      <c r="V10" s="76"/>
+      <c r="W10" s="73"/>
       <c r="X10" s="15"/>
-      <c r="Y10" s="85" t="s">
+      <c r="Y10" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="Z10" s="85"/>
-      <c r="AA10" s="85"/>
-      <c r="AB10" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC10" s="85"/>
-      <c r="AD10" s="82"/>
+      <c r="AC10" s="68"/>
+      <c r="AD10" s="69"/>
       <c r="AE10" s="16"/>
-      <c r="AF10" s="85" t="s">
+      <c r="AF10" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG10" s="68"/>
+      <c r="AH10" s="68"/>
+      <c r="AI10" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AG10" s="85"/>
-      <c r="AH10" s="85"/>
-      <c r="AI10" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ10" s="85"/>
-      <c r="AK10" s="82"/>
+      <c r="AJ10" s="68"/>
+      <c r="AK10" s="69"/>
       <c r="AL10" s="16"/>
-      <c r="AM10" s="85" t="s">
+      <c r="AM10" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN10" s="68"/>
+      <c r="AO10" s="68"/>
+      <c r="AP10" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="AN10" s="85"/>
-      <c r="AO10" s="85"/>
-      <c r="AP10" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ10" s="85"/>
-      <c r="AR10" s="82"/>
+      <c r="AQ10" s="68"/>
+      <c r="AR10" s="69"/>
       <c r="AS10" s="17"/>
-      <c r="AT10" s="84" t="s">
+      <c r="AT10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU10" s="68"/>
+      <c r="AV10" s="68"/>
+      <c r="AW10" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="AU10" s="85"/>
-      <c r="AV10" s="85"/>
-      <c r="AW10" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX10" s="83"/>
-      <c r="AY10" s="83"/>
-      <c r="AZ10" s="83"/>
-      <c r="BA10" s="84" t="s">
+      <c r="AX10" s="70"/>
+      <c r="AY10" s="70"/>
+      <c r="AZ10" s="70"/>
+      <c r="BA10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB10" s="68"/>
+      <c r="BC10" s="68"/>
+      <c r="BD10" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="BB10" s="85"/>
-      <c r="BC10" s="85"/>
-      <c r="BD10" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="BE10" s="83"/>
-      <c r="BF10" s="83"/>
-      <c r="BG10" s="83"/>
-      <c r="BH10" s="84" t="s">
+      <c r="BE10" s="70"/>
+      <c r="BF10" s="70"/>
+      <c r="BG10" s="70"/>
+      <c r="BH10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI10" s="68"/>
+      <c r="BJ10" s="68"/>
+      <c r="BK10" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="BI10" s="85"/>
-      <c r="BJ10" s="85"/>
-      <c r="BK10" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="BL10" s="83"/>
-      <c r="BM10" s="83"/>
-      <c r="BN10" s="83"/>
-      <c r="BO10" s="84" t="s">
+      <c r="BL10" s="70"/>
+      <c r="BM10" s="70"/>
+      <c r="BN10" s="70"/>
+      <c r="BO10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="BP10" s="68"/>
+      <c r="BQ10" s="68"/>
+      <c r="BR10" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="BP10" s="85"/>
-      <c r="BQ10" s="85"/>
-      <c r="BR10" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="BS10" s="83"/>
-      <c r="BT10" s="83"/>
-      <c r="BU10" s="83"/>
+      <c r="BS10" s="70"/>
+      <c r="BT10" s="70"/>
+      <c r="BU10" s="70"/>
       <c r="BV10" s="9"/>
     </row>
     <row r="11" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="18">
         <v>1</v>
@@ -4629,7 +4630,7 @@
       </c>
       <c r="BV21" s="9"/>
     </row>
-    <row r="22" spans="2:74" s="88" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:74" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="39">
         <v>1</v>
       </c>
@@ -6828,7 +6829,7 @@
       </c>
       <c r="BV31" s="9"/>
     </row>
-    <row r="32" spans="2:74" s="88" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:74" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="39">
         <v>2</v>
       </c>
@@ -7920,10 +7921,10 @@
         <v>32.911392405063289</v>
       </c>
       <c r="BT36" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BU36" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BV36" s="9"/>
     </row>
@@ -9467,7 +9468,7 @@
       </c>
       <c r="BV43" s="9"/>
     </row>
-    <row r="44" spans="2:74" s="88" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:74" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="39">
         <v>3</v>
       </c>
@@ -13398,10 +13399,10 @@
         <v>17.480719794344473</v>
       </c>
       <c r="BM61" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BN61" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BO61" s="35">
         <v>293</v>
@@ -13416,17 +13417,17 @@
         <v>5.4607508532423212</v>
       </c>
       <c r="BS61" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BT61" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BU61" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BV61" s="9"/>
     </row>
-    <row r="62" spans="2:74" s="88" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:74" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="39">
         <v>4</v>
       </c>
@@ -13645,7 +13646,7 @@
         <v>43.002577319587637</v>
       </c>
     </row>
-    <row r="63" spans="2:74" s="88" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:74" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="39">
         <v>0</v>
       </c>
@@ -13940,50 +13941,50 @@
       <c r="BV64" s="55"/>
     </row>
     <row r="65" spans="3:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="87" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="87"/>
-      <c r="E65" s="87"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="87"/>
-      <c r="H65" s="87"/>
-      <c r="I65" s="87"/>
-      <c r="J65" s="87"/>
-      <c r="K65" s="87"/>
-      <c r="L65" s="87"/>
-      <c r="M65" s="87"/>
-      <c r="N65" s="87"/>
-      <c r="O65" s="89"/>
-      <c r="P65" s="89"/>
-      <c r="Q65" s="89"/>
-      <c r="R65" s="89"/>
-      <c r="S65" s="89"/>
-      <c r="T65" s="89"/>
-      <c r="U65" s="89"/>
-      <c r="V65" s="89"/>
-      <c r="W65" s="89"/>
-      <c r="X65" s="89"/>
-      <c r="Y65" s="89"/>
-      <c r="Z65" s="89"/>
-      <c r="AA65" s="89"/>
-      <c r="AB65" s="89"/>
-      <c r="AC65" s="89"/>
-      <c r="AD65" s="89"/>
-      <c r="AE65" s="89"/>
-      <c r="AF65" s="89"/>
-      <c r="AG65" s="89"/>
-      <c r="AH65" s="89"/>
-      <c r="AI65" s="89"/>
-      <c r="AJ65" s="89"/>
-      <c r="AK65" s="89"/>
-      <c r="AL65" s="89"/>
-      <c r="AM65" s="89"/>
-      <c r="AN65" s="89"/>
-      <c r="AO65" s="89"/>
-      <c r="AP65" s="89"/>
-      <c r="AQ65" s="89"/>
-      <c r="AR65" s="89"/>
+      <c r="C65" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="71"/>
+      <c r="K65" s="71"/>
+      <c r="L65" s="71"/>
+      <c r="M65" s="71"/>
+      <c r="N65" s="71"/>
+      <c r="O65" s="66"/>
+      <c r="P65" s="66"/>
+      <c r="Q65" s="66"/>
+      <c r="R65" s="66"/>
+      <c r="S65" s="66"/>
+      <c r="T65" s="66"/>
+      <c r="U65" s="66"/>
+      <c r="V65" s="66"/>
+      <c r="W65" s="66"/>
+      <c r="X65" s="66"/>
+      <c r="Y65" s="66"/>
+      <c r="Z65" s="66"/>
+      <c r="AA65" s="66"/>
+      <c r="AB65" s="66"/>
+      <c r="AC65" s="66"/>
+      <c r="AD65" s="66"/>
+      <c r="AE65" s="66"/>
+      <c r="AF65" s="66"/>
+      <c r="AG65" s="66"/>
+      <c r="AH65" s="66"/>
+      <c r="AI65" s="66"/>
+      <c r="AJ65" s="66"/>
+      <c r="AK65" s="66"/>
+      <c r="AL65" s="66"/>
+      <c r="AM65" s="66"/>
+      <c r="AN65" s="66"/>
+      <c r="AO65" s="66"/>
+      <c r="AP65" s="66"/>
+      <c r="AQ65" s="66"/>
+      <c r="AR65" s="66"/>
       <c r="AS65" s="56"/>
       <c r="AT65" s="57"/>
       <c r="AU65" s="58"/>
@@ -14047,7 +14048,7 @@
     </row>
     <row r="67" spans="3:52" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D67" s="61"/>
       <c r="E67" s="61"/>
@@ -14153,63 +14154,26 @@
     </row>
     <row r="69" spans="3:52" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="3:52" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="3:52" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="3:52" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="BO10:BQ10"/>
-    <mergeCell ref="BR10:BU10"/>
-    <mergeCell ref="AT10:AV10"/>
-    <mergeCell ref="AW10:AZ10"/>
-    <mergeCell ref="BA10:BC10"/>
-    <mergeCell ref="BD10:BG10"/>
-    <mergeCell ref="BH10:BJ10"/>
-    <mergeCell ref="BK10:BN10"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AB10:AD10"/>
-    <mergeCell ref="AF10:AH10"/>
-    <mergeCell ref="AI10:AK10"/>
-    <mergeCell ref="AM10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="C65:N65"/>
-    <mergeCell ref="BH8:BJ8"/>
-    <mergeCell ref="BK8:BN8"/>
-    <mergeCell ref="BO8:BQ8"/>
-    <mergeCell ref="BR8:BU8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="AM8:AO8"/>
-    <mergeCell ref="AP8:AS8"/>
-    <mergeCell ref="AT8:AV8"/>
-    <mergeCell ref="AW8:AZ8"/>
-    <mergeCell ref="BA8:BC8"/>
-    <mergeCell ref="BD8:BG8"/>
-    <mergeCell ref="BA7:BG7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="U8:X8"/>
-    <mergeCell ref="Y8:AA8"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="AF8:AH8"/>
     <mergeCell ref="BH7:BN7"/>
     <mergeCell ref="BO7:BU7"/>
     <mergeCell ref="B7:B10"/>
@@ -14226,6 +14190,43 @@
     <mergeCell ref="AF7:AL7"/>
     <mergeCell ref="AM7:AS7"/>
     <mergeCell ref="AT7:AZ7"/>
+    <mergeCell ref="BA7:BG7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="Y8:AA8"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="AF8:AH8"/>
+    <mergeCell ref="BR8:BU8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="AM8:AO8"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AT8:AV8"/>
+    <mergeCell ref="AW8:AZ8"/>
+    <mergeCell ref="BA8:BC8"/>
+    <mergeCell ref="BD8:BG8"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="C65:N65"/>
+    <mergeCell ref="BH8:BJ8"/>
+    <mergeCell ref="BK8:BN8"/>
+    <mergeCell ref="BO8:BQ8"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="AF10:AH10"/>
+    <mergeCell ref="AI10:AK10"/>
+    <mergeCell ref="AM10:AO10"/>
+    <mergeCell ref="BO10:BQ10"/>
+    <mergeCell ref="BR10:BU10"/>
+    <mergeCell ref="AT10:AV10"/>
+    <mergeCell ref="AW10:AZ10"/>
+    <mergeCell ref="BA10:BC10"/>
+    <mergeCell ref="BD10:BG10"/>
+    <mergeCell ref="BH10:BJ10"/>
+    <mergeCell ref="BK10:BN10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C72" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ e68a065452251d712c621cd281201c1306c1cefe 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_5-2-2.xlsx
+++ b/assets/excel/2021_5-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9300CCBF-8E72-4810-AA43-8EB3E5734C04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA173682-6DDA-47F5-ACE5-BF71AEF407CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,11 +122,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="###\ ###\ ##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="###\ ###\ ###.0"/>
     <numFmt numFmtId="167" formatCode="###\ ##0"/>
+    <numFmt numFmtId="168" formatCode="###\ ###\ ###"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -334,7 +335,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -512,36 +513,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,6 +551,42 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1668,222 +1675,222 @@
       <c r="BV6" s="9"/>
     </row>
     <row r="7" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="87">
+      <c r="D7" s="77">
         <v>2020</v>
       </c>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="87">
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="77">
         <v>2019</v>
       </c>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="89"/>
-      <c r="R7" s="87">
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="77">
         <v>2018</v>
       </c>
-      <c r="S7" s="88"/>
-      <c r="T7" s="88"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="88"/>
-      <c r="W7" s="88"/>
-      <c r="X7" s="89"/>
-      <c r="Y7" s="77">
+      <c r="S7" s="78"/>
+      <c r="T7" s="78"/>
+      <c r="U7" s="78"/>
+      <c r="V7" s="78"/>
+      <c r="W7" s="78"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="67">
         <v>2017</v>
       </c>
-      <c r="Z7" s="78"/>
-      <c r="AA7" s="78"/>
-      <c r="AB7" s="78"/>
-      <c r="AC7" s="78"/>
-      <c r="AD7" s="78"/>
-      <c r="AE7" s="79"/>
-      <c r="AF7" s="77">
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="68"/>
+      <c r="AD7" s="68"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="67">
         <v>2016</v>
       </c>
-      <c r="AG7" s="78"/>
-      <c r="AH7" s="78"/>
-      <c r="AI7" s="78"/>
-      <c r="AJ7" s="78"/>
-      <c r="AK7" s="78"/>
-      <c r="AL7" s="79"/>
-      <c r="AM7" s="77">
+      <c r="AG7" s="68"/>
+      <c r="AH7" s="68"/>
+      <c r="AI7" s="68"/>
+      <c r="AJ7" s="68"/>
+      <c r="AK7" s="68"/>
+      <c r="AL7" s="69"/>
+      <c r="AM7" s="67">
         <v>2015</v>
       </c>
-      <c r="AN7" s="78"/>
-      <c r="AO7" s="78"/>
-      <c r="AP7" s="78"/>
-      <c r="AQ7" s="78"/>
-      <c r="AR7" s="78"/>
-      <c r="AS7" s="79"/>
-      <c r="AT7" s="77">
+      <c r="AN7" s="68"/>
+      <c r="AO7" s="68"/>
+      <c r="AP7" s="68"/>
+      <c r="AQ7" s="68"/>
+      <c r="AR7" s="68"/>
+      <c r="AS7" s="69"/>
+      <c r="AT7" s="67">
         <v>2014</v>
       </c>
-      <c r="AU7" s="78"/>
-      <c r="AV7" s="78"/>
-      <c r="AW7" s="78"/>
-      <c r="AX7" s="78"/>
-      <c r="AY7" s="78"/>
-      <c r="AZ7" s="79"/>
-      <c r="BA7" s="77">
+      <c r="AU7" s="68"/>
+      <c r="AV7" s="68"/>
+      <c r="AW7" s="68"/>
+      <c r="AX7" s="68"/>
+      <c r="AY7" s="68"/>
+      <c r="AZ7" s="69"/>
+      <c r="BA7" s="67">
         <v>2013</v>
       </c>
-      <c r="BB7" s="78"/>
-      <c r="BC7" s="78"/>
-      <c r="BD7" s="78"/>
-      <c r="BE7" s="78"/>
-      <c r="BF7" s="78"/>
-      <c r="BG7" s="79"/>
-      <c r="BH7" s="77">
+      <c r="BB7" s="68"/>
+      <c r="BC7" s="68"/>
+      <c r="BD7" s="68"/>
+      <c r="BE7" s="68"/>
+      <c r="BF7" s="68"/>
+      <c r="BG7" s="69"/>
+      <c r="BH7" s="67">
         <v>2011</v>
       </c>
-      <c r="BI7" s="78"/>
-      <c r="BJ7" s="78"/>
-      <c r="BK7" s="78"/>
-      <c r="BL7" s="78"/>
-      <c r="BM7" s="78"/>
-      <c r="BN7" s="79"/>
-      <c r="BO7" s="80">
+      <c r="BI7" s="68"/>
+      <c r="BJ7" s="68"/>
+      <c r="BK7" s="68"/>
+      <c r="BL7" s="68"/>
+      <c r="BM7" s="68"/>
+      <c r="BN7" s="69"/>
+      <c r="BO7" s="70">
         <v>2010</v>
       </c>
-      <c r="BP7" s="80"/>
-      <c r="BQ7" s="80"/>
-      <c r="BR7" s="80"/>
-      <c r="BS7" s="80"/>
-      <c r="BT7" s="80"/>
-      <c r="BU7" s="77"/>
+      <c r="BP7" s="70"/>
+      <c r="BQ7" s="70"/>
+      <c r="BR7" s="70"/>
+      <c r="BS7" s="70"/>
+      <c r="BT7" s="70"/>
+      <c r="BU7" s="67"/>
       <c r="BV7" s="11"/>
     </row>
     <row r="8" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="82"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="73" t="s">
+      <c r="B8" s="72"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="74"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="73" t="s">
+      <c r="E8" s="81"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="76" t="s">
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="73" t="s">
+      <c r="L8" s="83"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="76" t="s">
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="73" t="s">
+      <c r="S8" s="83"/>
+      <c r="T8" s="83"/>
+      <c r="U8" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="75"/>
-      <c r="Y8" s="68" t="s">
+      <c r="V8" s="81"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="Z8" s="68"/>
-      <c r="AA8" s="68"/>
-      <c r="AB8" s="69" t="s">
+      <c r="Z8" s="87"/>
+      <c r="AA8" s="87"/>
+      <c r="AB8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AC8" s="70"/>
-      <c r="AD8" s="70"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="68" t="s">
+      <c r="AC8" s="85"/>
+      <c r="AD8" s="85"/>
+      <c r="AE8" s="86"/>
+      <c r="AF8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="AG8" s="68"/>
-      <c r="AH8" s="68"/>
-      <c r="AI8" s="69" t="s">
+      <c r="AG8" s="87"/>
+      <c r="AH8" s="87"/>
+      <c r="AI8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AJ8" s="70"/>
-      <c r="AK8" s="70"/>
-      <c r="AL8" s="67"/>
-      <c r="AM8" s="68" t="s">
+      <c r="AJ8" s="85"/>
+      <c r="AK8" s="85"/>
+      <c r="AL8" s="86"/>
+      <c r="AM8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="AN8" s="68"/>
-      <c r="AO8" s="68"/>
-      <c r="AP8" s="69" t="s">
+      <c r="AN8" s="87"/>
+      <c r="AO8" s="87"/>
+      <c r="AP8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AQ8" s="70"/>
-      <c r="AR8" s="70"/>
-      <c r="AS8" s="67"/>
-      <c r="AT8" s="68" t="s">
+      <c r="AQ8" s="85"/>
+      <c r="AR8" s="85"/>
+      <c r="AS8" s="86"/>
+      <c r="AT8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="AU8" s="68"/>
-      <c r="AV8" s="68"/>
-      <c r="AW8" s="69" t="s">
+      <c r="AU8" s="87"/>
+      <c r="AV8" s="87"/>
+      <c r="AW8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AX8" s="70"/>
-      <c r="AY8" s="70"/>
-      <c r="AZ8" s="67"/>
-      <c r="BA8" s="68" t="s">
+      <c r="AX8" s="85"/>
+      <c r="AY8" s="85"/>
+      <c r="AZ8" s="86"/>
+      <c r="BA8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="BB8" s="68"/>
-      <c r="BC8" s="68"/>
-      <c r="BD8" s="69" t="s">
+      <c r="BB8" s="87"/>
+      <c r="BC8" s="87"/>
+      <c r="BD8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="BE8" s="70"/>
-      <c r="BF8" s="70"/>
-      <c r="BG8" s="67"/>
-      <c r="BH8" s="68" t="s">
+      <c r="BE8" s="85"/>
+      <c r="BF8" s="85"/>
+      <c r="BG8" s="86"/>
+      <c r="BH8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="BI8" s="68"/>
-      <c r="BJ8" s="68"/>
-      <c r="BK8" s="69" t="s">
+      <c r="BI8" s="87"/>
+      <c r="BJ8" s="87"/>
+      <c r="BK8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="BL8" s="70"/>
-      <c r="BM8" s="70"/>
-      <c r="BN8" s="67"/>
-      <c r="BO8" s="72" t="s">
+      <c r="BL8" s="85"/>
+      <c r="BM8" s="85"/>
+      <c r="BN8" s="86"/>
+      <c r="BO8" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="BP8" s="72"/>
-      <c r="BQ8" s="72"/>
-      <c r="BR8" s="69" t="s">
+      <c r="BP8" s="89"/>
+      <c r="BQ8" s="89"/>
+      <c r="BR8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="BS8" s="70"/>
-      <c r="BT8" s="70"/>
-      <c r="BU8" s="70"/>
+      <c r="BS8" s="85"/>
+      <c r="BT8" s="85"/>
+      <c r="BU8" s="85"/>
       <c r="BV8" s="9"/>
     </row>
     <row r="9" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="82"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2097,118 +2104,118 @@
       <c r="BV9" s="9"/>
     </row>
     <row r="10" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="83"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="73" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="74"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="73" t="s">
+      <c r="E10" s="81"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="76" t="s">
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76" t="s">
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="O10" s="76"/>
-      <c r="P10" s="73"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="80"/>
       <c r="Q10" s="15"/>
-      <c r="R10" s="76" t="s">
+      <c r="R10" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="76" t="s">
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="V10" s="76"/>
-      <c r="W10" s="73"/>
+      <c r="V10" s="83"/>
+      <c r="W10" s="80"/>
       <c r="X10" s="15"/>
-      <c r="Y10" s="68" t="s">
+      <c r="Y10" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="Z10" s="68"/>
-      <c r="AA10" s="68"/>
-      <c r="AB10" s="68" t="s">
+      <c r="Z10" s="87"/>
+      <c r="AA10" s="87"/>
+      <c r="AB10" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="AC10" s="68"/>
-      <c r="AD10" s="69"/>
+      <c r="AC10" s="87"/>
+      <c r="AD10" s="84"/>
       <c r="AE10" s="16"/>
-      <c r="AF10" s="68" t="s">
+      <c r="AF10" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="AG10" s="68"/>
-      <c r="AH10" s="68"/>
-      <c r="AI10" s="68" t="s">
+      <c r="AG10" s="87"/>
+      <c r="AH10" s="87"/>
+      <c r="AI10" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="AJ10" s="68"/>
-      <c r="AK10" s="69"/>
+      <c r="AJ10" s="87"/>
+      <c r="AK10" s="84"/>
       <c r="AL10" s="16"/>
-      <c r="AM10" s="68" t="s">
+      <c r="AM10" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="AN10" s="68"/>
-      <c r="AO10" s="68"/>
-      <c r="AP10" s="68" t="s">
+      <c r="AN10" s="87"/>
+      <c r="AO10" s="87"/>
+      <c r="AP10" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="AQ10" s="68"/>
-      <c r="AR10" s="69"/>
+      <c r="AQ10" s="87"/>
+      <c r="AR10" s="84"/>
       <c r="AS10" s="17"/>
-      <c r="AT10" s="67" t="s">
+      <c r="AT10" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AU10" s="68"/>
-      <c r="AV10" s="68"/>
-      <c r="AW10" s="69" t="s">
+      <c r="AU10" s="87"/>
+      <c r="AV10" s="87"/>
+      <c r="AW10" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="AX10" s="70"/>
-      <c r="AY10" s="70"/>
-      <c r="AZ10" s="70"/>
-      <c r="BA10" s="67" t="s">
+      <c r="AX10" s="85"/>
+      <c r="AY10" s="85"/>
+      <c r="AZ10" s="85"/>
+      <c r="BA10" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="BB10" s="68"/>
-      <c r="BC10" s="68"/>
-      <c r="BD10" s="69" t="s">
+      <c r="BB10" s="87"/>
+      <c r="BC10" s="87"/>
+      <c r="BD10" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="BE10" s="70"/>
-      <c r="BF10" s="70"/>
-      <c r="BG10" s="70"/>
-      <c r="BH10" s="67" t="s">
+      <c r="BE10" s="85"/>
+      <c r="BF10" s="85"/>
+      <c r="BG10" s="85"/>
+      <c r="BH10" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="BI10" s="68"/>
-      <c r="BJ10" s="68"/>
-      <c r="BK10" s="69" t="s">
+      <c r="BI10" s="87"/>
+      <c r="BJ10" s="87"/>
+      <c r="BK10" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="BL10" s="70"/>
-      <c r="BM10" s="70"/>
-      <c r="BN10" s="70"/>
-      <c r="BO10" s="67" t="s">
+      <c r="BL10" s="85"/>
+      <c r="BM10" s="85"/>
+      <c r="BN10" s="85"/>
+      <c r="BO10" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="BP10" s="68"/>
-      <c r="BQ10" s="68"/>
-      <c r="BR10" s="69" t="s">
+      <c r="BP10" s="87"/>
+      <c r="BQ10" s="87"/>
+      <c r="BR10" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="BS10" s="70"/>
-      <c r="BT10" s="70"/>
-      <c r="BU10" s="70"/>
+      <c r="BS10" s="85"/>
+      <c r="BT10" s="85"/>
+      <c r="BU10" s="85"/>
       <c r="BV10" s="9"/>
     </row>
     <row r="11" spans="2:74" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2438,13 +2445,13 @@
         <f>VLOOKUP(B12,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Braunschweig  Stadt</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="90">
         <v>11541</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="90">
         <v>6997</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="90">
         <v>4544</v>
       </c>
       <c r="G12" s="21">
@@ -2658,13 +2665,13 @@
         <f>VLOOKUP(B13,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Salzgitter  Stadt</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="90">
         <v>4878</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="90">
         <v>3738</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="90">
         <v>1140</v>
       </c>
       <c r="G13" s="21">
@@ -2878,13 +2885,13 @@
         <f>VLOOKUP(B14,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Wolfsburg  Stadt</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="90">
         <v>10661</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="90">
         <v>7333</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="90">
         <v>3328</v>
       </c>
       <c r="G14" s="21">
@@ -3098,13 +3105,13 @@
         <f>VLOOKUP(B15,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Gifhorn</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="90">
         <v>3257</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="90">
         <v>2169</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="90">
         <v>1088</v>
       </c>
       <c r="G15" s="21">
@@ -3318,13 +3325,13 @@
         <f>VLOOKUP(B16,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Goslar</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="90">
         <v>3225</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="90">
         <v>2090</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="90">
         <v>1135</v>
       </c>
       <c r="G16" s="21">
@@ -3538,13 +3545,13 @@
         <f>VLOOKUP(B17,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Helmstedt</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="90">
         <v>1701</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="90">
         <v>1149</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="90">
         <v>552</v>
       </c>
       <c r="G17" s="21">
@@ -3758,13 +3765,13 @@
         <f>VLOOKUP(B18,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Northeim</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="90">
         <v>3416</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="90">
         <v>2534</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="90">
         <v>882</v>
       </c>
       <c r="G18" s="21">
@@ -3978,13 +3985,13 @@
         <f>VLOOKUP(B19,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Peine</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="90">
         <v>3368</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="90">
         <v>2434</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="90">
         <v>934</v>
       </c>
       <c r="G19" s="21">
@@ -4198,13 +4205,13 @@
         <f>VLOOKUP(B20,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Wolfenbüttel</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="90">
         <v>1586</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="90">
         <v>1010</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="90">
         <v>576</v>
       </c>
       <c r="G20" s="21">
@@ -4418,13 +4425,13 @@
         <f>VLOOKUP(B21,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Göttingen</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="90">
         <v>9833</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="90">
         <v>6074</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="90">
         <v>3759</v>
       </c>
       <c r="G21" s="21">
@@ -4638,13 +4645,13 @@
         <f>VLOOKUP(B22,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Statistische Region Braunschweig</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="91">
         <v>53466</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="91">
         <v>35528</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="91">
         <v>17938</v>
       </c>
       <c r="G22" s="42">
@@ -4857,13 +4864,13 @@
         <f>VLOOKUP(B23,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Hannover  Region</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="90">
         <v>62632</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="90">
         <v>38889</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="90">
         <v>23743</v>
       </c>
       <c r="G23" s="21">
@@ -5077,13 +5084,13 @@
         <f>VLOOKUP(B24,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>dav. Hannover  Lhst.</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="90">
         <v>38815</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="90">
         <v>22979</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="90">
         <v>15836</v>
       </c>
       <c r="G24" s="21">
@@ -5297,13 +5304,13 @@
         <f>VLOOKUP(B25,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>dav. Hannover  Umland</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="90">
         <v>23817</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="90">
         <v>15910</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="90">
         <v>7907</v>
       </c>
       <c r="G25" s="21">
@@ -5517,13 +5524,13 @@
         <f>VLOOKUP(B26,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Diepholz</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="90">
         <v>6594</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="90">
         <v>4544</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="90">
         <v>2050</v>
       </c>
       <c r="G26" s="21">
@@ -5737,13 +5744,13 @@
         <f>VLOOKUP(B27,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Hameln-Pyrmont</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="90">
         <v>4124</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="90">
         <v>2541</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="90">
         <v>1583</v>
       </c>
       <c r="G27" s="21">
@@ -5957,13 +5964,13 @@
         <f>VLOOKUP(B28,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Hildesheim</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="90">
         <v>6461</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="90">
         <v>4211</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="90">
         <v>2250</v>
       </c>
       <c r="G28" s="21">
@@ -6177,13 +6184,13 @@
         <f>VLOOKUP(B29,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Holzminden</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="90">
         <v>1484</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="90">
         <v>998</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="90">
         <v>486</v>
       </c>
       <c r="G29" s="21">
@@ -6397,13 +6404,13 @@
         <f>VLOOKUP(B30,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Nienburg (Weser)</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="90">
         <v>4349</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="90">
         <v>3022</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="90">
         <v>1327</v>
       </c>
       <c r="G30" s="21">
@@ -6617,13 +6624,13 @@
         <f>VLOOKUP(B31,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Schaumburg</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="90">
         <v>3862</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="90">
         <v>2539</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="90">
         <v>1323</v>
       </c>
       <c r="G31" s="21">
@@ -6837,13 +6844,13 @@
         <f>VLOOKUP(B32,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Statistische Region Hannover</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="91">
         <v>89506</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="91">
         <v>56744</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="91">
         <v>32762</v>
       </c>
       <c r="G32" s="42">
@@ -7056,13 +7063,13 @@
         <f>VLOOKUP(B33,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Celle</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="90">
         <v>4092</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="90">
         <v>2631</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="90">
         <v>1461</v>
       </c>
       <c r="G33" s="21">
@@ -7276,13 +7283,13 @@
         <f>VLOOKUP(B34,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Cuxhaven</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="90">
         <v>4388</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="90">
         <v>2924</v>
       </c>
-      <c r="F34" s="20">
+      <c r="F34" s="90">
         <v>1464</v>
       </c>
       <c r="G34" s="21">
@@ -7496,13 +7503,13 @@
         <f>VLOOKUP(B35,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Harburg</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="90">
         <v>9737</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="90">
         <v>7051</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="90">
         <v>2686</v>
       </c>
       <c r="G35" s="21">
@@ -7716,13 +7723,13 @@
         <f>VLOOKUP(B36,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Lüchow-Dannenberg</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D36" s="90">
         <v>750</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="90">
         <v>456</v>
       </c>
-      <c r="F36" s="20">
+      <c r="F36" s="90">
         <v>294</v>
       </c>
       <c r="G36" s="21">
@@ -7936,13 +7943,13 @@
         <f>VLOOKUP(B37,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Lüneburg</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="90">
         <v>3926</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="90">
         <v>2530</v>
       </c>
-      <c r="F37" s="20">
+      <c r="F37" s="90">
         <v>1396</v>
       </c>
       <c r="G37" s="21">
@@ -8156,13 +8163,13 @@
         <f>VLOOKUP(B38,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Osterholz</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="90">
         <v>2020</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="90">
         <v>1391</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="90">
         <v>629</v>
       </c>
       <c r="G38" s="21">
@@ -8376,13 +8383,13 @@
         <f>VLOOKUP(B39,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Rotenburg (Wümme)</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D39" s="90">
         <v>4630</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E39" s="90">
         <v>3136</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="90">
         <v>1494</v>
       </c>
       <c r="G39" s="21">
@@ -8596,13 +8603,13 @@
         <f>VLOOKUP(B40,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Heidekreis</v>
       </c>
-      <c r="D40" s="20">
+      <c r="D40" s="90">
         <v>4303</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="90">
         <v>2824</v>
       </c>
-      <c r="F40" s="20">
+      <c r="F40" s="90">
         <v>1479</v>
       </c>
       <c r="G40" s="21">
@@ -8816,13 +8823,13 @@
         <f>VLOOKUP(B41,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Stade</v>
       </c>
-      <c r="D41" s="20">
+      <c r="D41" s="90">
         <v>5874</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="90">
         <v>4173</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="90">
         <v>1701</v>
       </c>
       <c r="G41" s="21">
@@ -9036,13 +9043,13 @@
         <f>VLOOKUP(B42,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Uelzen</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="90">
         <v>1682</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="90">
         <v>1035</v>
       </c>
-      <c r="F42" s="20">
+      <c r="F42" s="90">
         <v>647</v>
       </c>
       <c r="G42" s="21">
@@ -9256,13 +9263,13 @@
         <f>VLOOKUP(B43,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Verden</v>
       </c>
-      <c r="D43" s="20">
+      <c r="D43" s="90">
         <v>5629</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="90">
         <v>3944</v>
       </c>
-      <c r="F43" s="20">
+      <c r="F43" s="90">
         <v>1685</v>
       </c>
       <c r="G43" s="21">
@@ -9476,13 +9483,13 @@
         <f>VLOOKUP(B44,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Statistische Region Lüneburg</v>
       </c>
-      <c r="D44" s="40">
+      <c r="D44" s="91">
         <v>47031</v>
       </c>
-      <c r="E44" s="40">
+      <c r="E44" s="91">
         <v>32095</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="91">
         <v>14936</v>
       </c>
       <c r="G44" s="42">
@@ -9695,13 +9702,13 @@
         <f>VLOOKUP(B45,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Delmenhorst  Stadt</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="90">
         <v>1864</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="90">
         <v>1219</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F45" s="90">
         <v>645</v>
       </c>
       <c r="G45" s="21">
@@ -9915,13 +9922,13 @@
         <f>VLOOKUP(B46,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Emden  Stadt</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D46" s="90">
         <v>1823</v>
       </c>
-      <c r="E46" s="20">
+      <c r="E46" s="90">
         <v>1350</v>
       </c>
-      <c r="F46" s="20">
+      <c r="F46" s="90">
         <v>473</v>
       </c>
       <c r="G46" s="21">
@@ -10135,13 +10142,13 @@
         <f>VLOOKUP(B47,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Oldenburg(Oldb)  Stadt</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D47" s="90">
         <v>6162</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="90">
         <v>3917</v>
       </c>
-      <c r="F47" s="20">
+      <c r="F47" s="90">
         <v>2245</v>
       </c>
       <c r="G47" s="21">
@@ -10355,13 +10362,13 @@
         <f>VLOOKUP(B48,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Osnabrück  Stadt</v>
       </c>
-      <c r="D48" s="20">
+      <c r="D48" s="90">
         <v>8847</v>
       </c>
-      <c r="E48" s="20">
+      <c r="E48" s="90">
         <v>4934</v>
       </c>
-      <c r="F48" s="20">
+      <c r="F48" s="90">
         <v>3913</v>
       </c>
       <c r="G48" s="21">
@@ -10575,13 +10582,13 @@
         <f>VLOOKUP(B49,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Wilhelmshaven  Stadt</v>
       </c>
-      <c r="D49" s="20">
+      <c r="D49" s="90">
         <v>1855</v>
       </c>
-      <c r="E49" s="20">
+      <c r="E49" s="90">
         <v>1310</v>
       </c>
-      <c r="F49" s="20">
+      <c r="F49" s="90">
         <v>545</v>
       </c>
       <c r="G49" s="21">
@@ -10795,13 +10802,13 @@
         <f>VLOOKUP(B50,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Ammerland</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D50" s="90">
         <v>4153</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="90">
         <v>2852</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="90">
         <v>1301</v>
       </c>
       <c r="G50" s="21">
@@ -11015,13 +11022,13 @@
         <f>VLOOKUP(B51,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Aurich</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="90">
         <v>4164</v>
       </c>
-      <c r="E51" s="20">
+      <c r="E51" s="90">
         <v>2658</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="90">
         <v>1506</v>
       </c>
       <c r="G51" s="21">
@@ -11235,13 +11242,13 @@
         <f>VLOOKUP(B52,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Cloppenburg</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="90">
         <v>10632</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="90">
         <v>7314</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="90">
         <v>3318</v>
       </c>
       <c r="G52" s="21">
@@ -11455,13 +11462,13 @@
         <f>VLOOKUP(B53,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Emsland</v>
       </c>
-      <c r="D53" s="20">
+      <c r="D53" s="90">
         <v>14967</v>
       </c>
-      <c r="E53" s="20">
+      <c r="E53" s="90">
         <v>10881</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="90">
         <v>4086</v>
       </c>
       <c r="G53" s="21">
@@ -11675,13 +11682,13 @@
         <f>VLOOKUP(B54,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Friesland</v>
       </c>
-      <c r="D54" s="20">
+      <c r="D54" s="90">
         <v>1524</v>
       </c>
-      <c r="E54" s="20">
+      <c r="E54" s="90">
         <v>982</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="90">
         <v>542</v>
       </c>
       <c r="G54" s="21">
@@ -11895,13 +11902,13 @@
         <f>VLOOKUP(B55,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Grafschaft Bentheim</v>
       </c>
-      <c r="D55" s="20">
+      <c r="D55" s="90">
         <v>5790</v>
       </c>
-      <c r="E55" s="20">
+      <c r="E55" s="90">
         <v>3984</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="90">
         <v>1806</v>
       </c>
       <c r="G55" s="21">
@@ -12115,13 +12122,13 @@
         <f>VLOOKUP(B56,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Leer</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="90">
         <v>3766</v>
       </c>
-      <c r="E56" s="20">
+      <c r="E56" s="90">
         <v>2684</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="90">
         <v>1082</v>
       </c>
       <c r="G56" s="21">
@@ -12335,13 +12342,13 @@
         <f>VLOOKUP(B57,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Oldenburg</v>
       </c>
-      <c r="D57" s="20">
+      <c r="D57" s="90">
         <v>3842</v>
       </c>
-      <c r="E57" s="20">
+      <c r="E57" s="90">
         <v>2708</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="90">
         <v>1134</v>
       </c>
       <c r="G57" s="21">
@@ -12555,13 +12562,13 @@
         <f>VLOOKUP(B58,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Osnabrück</v>
       </c>
-      <c r="D58" s="20">
+      <c r="D58" s="90">
         <v>17707</v>
       </c>
-      <c r="E58" s="20">
+      <c r="E58" s="90">
         <v>11697</v>
       </c>
-      <c r="F58" s="20">
+      <c r="F58" s="90">
         <v>6010</v>
       </c>
       <c r="G58" s="21">
@@ -12775,13 +12782,13 @@
         <f>VLOOKUP(B59,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Vechta</v>
       </c>
-      <c r="D59" s="20">
+      <c r="D59" s="90">
         <v>11205</v>
       </c>
-      <c r="E59" s="20">
+      <c r="E59" s="90">
         <v>7462</v>
       </c>
-      <c r="F59" s="20">
+      <c r="F59" s="90">
         <v>3743</v>
       </c>
       <c r="G59" s="21">
@@ -12995,13 +13002,13 @@
         <f>VLOOKUP(B60,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Wesermarsch</v>
       </c>
-      <c r="D60" s="20">
+      <c r="D60" s="90">
         <v>2505</v>
       </c>
-      <c r="E60" s="20">
+      <c r="E60" s="90">
         <v>1989</v>
       </c>
-      <c r="F60" s="20">
+      <c r="F60" s="90">
         <v>516</v>
       </c>
       <c r="G60" s="21">
@@ -13215,13 +13222,13 @@
         <f>VLOOKUP(B61,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Wittmund</v>
       </c>
-      <c r="D61" s="20">
+      <c r="D61" s="90">
         <v>924</v>
       </c>
-      <c r="E61" s="20">
+      <c r="E61" s="90">
         <v>546</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F61" s="90">
         <v>378</v>
       </c>
       <c r="G61" s="21">
@@ -13435,13 +13442,13 @@
         <f>VLOOKUP(B62,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Statistische Region Weser-Ems</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="91">
         <v>101730</v>
       </c>
-      <c r="E62" s="40">
+      <c r="E62" s="91">
         <v>68487</v>
       </c>
-      <c r="F62" s="40">
+      <c r="F62" s="91">
         <v>33243</v>
       </c>
       <c r="G62" s="42">
@@ -13654,13 +13661,13 @@
         <f>VLOOKUP(B63,[1]Tabelle1!$A$1:$B$68,2,FALSE)</f>
         <v>Niedersachsen</v>
       </c>
-      <c r="D63" s="40">
+      <c r="D63" s="91">
         <v>291733</v>
       </c>
-      <c r="E63" s="40">
+      <c r="E63" s="91">
         <v>192854</v>
       </c>
-      <c r="F63" s="40">
+      <c r="F63" s="91">
         <v>93737</v>
       </c>
       <c r="G63" s="42">
@@ -13941,20 +13948,20 @@
       <c r="BV64" s="55"/>
     </row>
     <row r="65" spans="3:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="71" t="s">
+      <c r="C65" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
-      <c r="F65" s="71"/>
-      <c r="G65" s="71"/>
-      <c r="H65" s="71"/>
-      <c r="I65" s="71"/>
-      <c r="J65" s="71"/>
-      <c r="K65" s="71"/>
-      <c r="L65" s="71"/>
-      <c r="M65" s="71"/>
-      <c r="N65" s="71"/>
+      <c r="D65" s="88"/>
+      <c r="E65" s="88"/>
+      <c r="F65" s="88"/>
+      <c r="G65" s="88"/>
+      <c r="H65" s="88"/>
+      <c r="I65" s="88"/>
+      <c r="J65" s="88"/>
+      <c r="K65" s="88"/>
+      <c r="L65" s="88"/>
+      <c r="M65" s="88"/>
+      <c r="N65" s="88"/>
       <c r="O65" s="66"/>
       <c r="P65" s="66"/>
       <c r="Q65" s="66"/>
@@ -14174,6 +14181,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="C65:N65"/>
+    <mergeCell ref="BH8:BJ8"/>
+    <mergeCell ref="BK8:BN8"/>
+    <mergeCell ref="BO8:BQ8"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="AF10:AH10"/>
+    <mergeCell ref="AI10:AK10"/>
+    <mergeCell ref="AM10:AO10"/>
+    <mergeCell ref="BO10:BQ10"/>
+    <mergeCell ref="AT10:AV10"/>
+    <mergeCell ref="AW10:AZ10"/>
+    <mergeCell ref="BA10:BC10"/>
+    <mergeCell ref="BD10:BG10"/>
+    <mergeCell ref="BH10:BJ10"/>
+    <mergeCell ref="BK10:BN10"/>
+    <mergeCell ref="BR8:BU8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="AM8:AO8"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AT8:AV8"/>
+    <mergeCell ref="AW8:AZ8"/>
+    <mergeCell ref="BA8:BC8"/>
+    <mergeCell ref="BD8:BG8"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="BR10:BU10"/>
+    <mergeCell ref="BA7:BG7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="Y8:AA8"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="AF8:AH8"/>
     <mergeCell ref="BH7:BN7"/>
     <mergeCell ref="BO7:BU7"/>
     <mergeCell ref="B7:B10"/>
@@ -14190,43 +14234,6 @@
     <mergeCell ref="AF7:AL7"/>
     <mergeCell ref="AM7:AS7"/>
     <mergeCell ref="AT7:AZ7"/>
-    <mergeCell ref="BA7:BG7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="U8:X8"/>
-    <mergeCell ref="Y8:AA8"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="AF8:AH8"/>
-    <mergeCell ref="BR8:BU8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="AM8:AO8"/>
-    <mergeCell ref="AP8:AS8"/>
-    <mergeCell ref="AT8:AV8"/>
-    <mergeCell ref="AW8:AZ8"/>
-    <mergeCell ref="BA8:BC8"/>
-    <mergeCell ref="BD8:BG8"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="C65:N65"/>
-    <mergeCell ref="BH8:BJ8"/>
-    <mergeCell ref="BK8:BN8"/>
-    <mergeCell ref="BO8:BQ8"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AB10:AD10"/>
-    <mergeCell ref="AF10:AH10"/>
-    <mergeCell ref="AI10:AK10"/>
-    <mergeCell ref="AM10:AO10"/>
-    <mergeCell ref="BO10:BQ10"/>
-    <mergeCell ref="BR10:BU10"/>
-    <mergeCell ref="AT10:AV10"/>
-    <mergeCell ref="AW10:AZ10"/>
-    <mergeCell ref="BA10:BC10"/>
-    <mergeCell ref="BD10:BG10"/>
-    <mergeCell ref="BH10:BJ10"/>
-    <mergeCell ref="BK10:BN10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C72" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>